<commit_message>
bug fix for robot size more than the grid size
</commit_message>
<xml_diff>
--- a/Data/maps/map16x22.xlsx
+++ b/Data/maps/map16x22.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stummuac-my.sharepoint.com/personal/55141653_ad_mmu_ac_uk/Documents/Documents/ubuntu/occupancy-grid-a-star-master/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\rumy\python-projects\Assignment\project\Data\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="132" documentId="11_F25DC773A252ABDACC1048C901DB407A5ADE58EA" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C5E9020B-1B72-4C9C-B228-783853244C8B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F82C15A-C519-40E3-9356-80F6893EE4DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -340,7 +340,7 @@
   <dimension ref="A1:P22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,13 +524,13 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4">
         <v>0</v>

</xml_diff>